<commit_message>
Criacao da database RLSalesDB e das tabelas TB_Order e TB_OrderItem
</commit_message>
<xml_diff>
--- a/SaleManagement/venda.xlsx
+++ b/SaleManagement/venda.xlsx
@@ -16,48 +16,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>Venda</t>
-  </si>
-  <si>
-    <t>codigo</t>
-  </si>
-  <si>
-    <t>serial</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>primary key</t>
   </si>
   <si>
-    <t>produto</t>
-  </si>
-  <si>
-    <t>cliente</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
-    <t>valor_total</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>data_venda</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>notnull</t>
   </si>
   <si>
-    <t>qtd</t>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>OrderItem</t>
+  </si>
+  <si>
+    <t>CustomerId</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>decimal(14,2)</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>PaymentForm</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>UnitValue</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>RLSalesDB</t>
   </si>
 </sst>
 </file>
@@ -396,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,71 +434,141 @@
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criacao da procedure de consulta das tabelas order e order item
</commit_message>
<xml_diff>
--- a/SaleManagement/venda.xlsx
+++ b/SaleManagement/venda.xlsx
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>